<commit_message>
Framework auf 4.6.1 ändern
</commit_message>
<xml_diff>
--- a/Dokumentation/Aufgaben.xlsx
+++ b/Dokumentation/Aufgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SmartFridge\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24C5ACF7-ACFB-4140-8770-AF422B9B1D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A72297-AFAE-4A5C-A68B-16390E23DF5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{38353211-F5DA-4C89-BC1D-2601A6056858}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{38353211-F5DA-4C89-BC1D-2601A6056858}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Barcodes</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Bilder</t>
   </si>
   <si>
-    <t>Dateisystem für Bilder, Product::ImagePath, ProductForm &amp; ProductOverview: Bild anzeigen</t>
-  </si>
-  <si>
     <t>Filter ProductOverview</t>
   </si>
   <si>
@@ -97,6 +94,21 @@
   </si>
   <si>
     <t>Datenbank füllen</t>
+  </si>
+  <si>
+    <t>Sonstiges</t>
+  </si>
+  <si>
+    <t>Dateisystem für Bilder, Product::ImageId, ProductForm &amp; ProductOverview: Bild anzeigen</t>
+  </si>
+  <si>
+    <t>Julius</t>
+  </si>
+  <si>
+    <t>Produktdatenbank mit Infos und Bildern füllen</t>
+  </si>
+  <si>
+    <t>BWLer</t>
   </si>
 </sst>
 </file>
@@ -172,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -190,6 +202,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -504,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2C5B32-801C-4E7E-B757-77972647774B}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +532,7 @@
     <col min="2" max="2" width="94.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -533,14 +549,18 @@
         <v>3</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -553,31 +573,35 @@
         <v>4</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -587,10 +611,11 @@
         <v>4</v>
       </c>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -598,10 +623,11 @@
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -609,13 +635,14 @@
       <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -623,13 +650,14 @@
         <v>4</v>
       </c>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -637,47 +665,68 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aufgaben nach Priorität sortiert
</commit_message>
<xml_diff>
--- a/Dokumentation/Aufgaben.xlsx
+++ b/Dokumentation/Aufgaben.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SmartFridge\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997E97B1-9D69-4414-880C-B9F28A45842E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24C5ACF7-ACFB-4140-8770-AF422B9B1D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{38353211-F5DA-4C89-BC1D-2601A6056858}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{38353211-F5DA-4C89-BC1D-2601A6056858}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Barcodes</t>
   </si>
@@ -60,6 +60,9 @@
     <t>Bilder</t>
   </si>
   <si>
+    <t>Dateisystem für Bilder, Product::ImagePath, ProductForm &amp; ProductOverview: Bild anzeigen</t>
+  </si>
+  <si>
     <t>Filter ProductOverview</t>
   </si>
   <si>
@@ -94,33 +97,6 @@
   </si>
   <si>
     <t>Datenbank füllen</t>
-  </si>
-  <si>
-    <t>Sonstiges</t>
-  </si>
-  <si>
-    <t>Dateisystem für Bilder, Product::ImageId, ProductForm &amp; ProductOverview: Bild anzeigen</t>
-  </si>
-  <si>
-    <t>Julius</t>
-  </si>
-  <si>
-    <t>Produktdatenbank mit Infos und Bildern füllen</t>
-  </si>
-  <si>
-    <t>BWLer</t>
-  </si>
-  <si>
-    <t>Nils, Janni</t>
-  </si>
-  <si>
-    <t>Ugur</t>
-  </si>
-  <si>
-    <t>Lokaler Datencache</t>
-  </si>
-  <si>
-    <t>Cache für Datenbank und Bilder, synchronisiert alle 5 min., puffert DB und Bilder für Offlinefunktionalität</t>
   </si>
 </sst>
 </file>
@@ -196,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -214,10 +190,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -532,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2C5B32-801C-4E7E-B757-77972647774B}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +516,7 @@
     <col min="2" max="2" width="94.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -561,18 +533,14 @@
         <v>3</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -585,14 +553,13 @@
         <v>4</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -604,16 +571,13 @@
         <v>4</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
@@ -623,13 +587,10 @@
         <v>4</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -637,11 +598,10 @@
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -649,14 +609,13 @@
       <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -664,16 +623,13 @@
         <v>4</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -681,81 +637,47 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
     </row>
   </sheetData>

</xml_diff>